<commit_message>
updates for compositional analysis
</commit_message>
<xml_diff>
--- a/biorefineries/cane/data/cane_composition_data.xlsx
+++ b/biorefineries/cane/data/cane_composition_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\biosteam\Bioindustrial-Park\biorefineries\cane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E32E68-DD39-4E3D-95D0-37D195D60BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB502FE-AF9B-422E-9690-A28741E49167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A4D5F0FC-4525-4FC3-8D16-C4CDE02F4321}"/>
   </bookViews>
@@ -205,9 +205,6 @@
     <t>Energy cane (Louisiana)</t>
   </si>
   <si>
-    <t>Yield (MT/hc)</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -239,12 +236,18 @@
   </si>
   <si>
     <t>Biomass yield (dry MT/hc)</t>
+  </si>
+  <si>
+    <t>Yield (dry MT/hc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,10 +295,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -310,16 +314,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -626,7 +631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,7 +642,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,36 +662,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="6"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -728,51 +733,51 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <f>1 - D3 - F3 - 0.07</f>
         <v>0.48698388391867048</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <f>AVERAGE('Raw data'!G3, 'Raw data'!G7, 'Raw data'!H3, 'Raw data'!H7) / 100 / 'Raw data'!$C$26</f>
         <v>3.9314599966733151E-3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <f>AVERAGE('Raw data'!G3, 'Raw data'!G7)  / 100 / 'Raw data'!$C$26- D3</f>
         <v>4.8418787425149722E-4</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <f>AVERAGE('Raw data'!E3, 'Raw data'!E7) * H3 / (1 - H3) / 100</f>
         <v>0.43908465608465613</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <f>AVERAGE('Raw data'!F3, 'Raw data'!F7) * I3 / (1 - I3) / 100</f>
         <v>3.9848484848484842E-5</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <f>AVERAGE('Raw data'!C3, 'Raw data'!C7) + 0.55 * (1 -  AVERAGE('Raw data'!C3, 'Raw data'!C7))</f>
         <v>0.66925000000000001</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <f>AVERAGE('Raw data'!D3, 'Raw data'!D7)</f>
         <v>0.01</v>
       </c>
-      <c r="J3" s="9">
-        <f>L3*'Raw data'!$F$25</f>
-        <v>19.44650602409639</v>
-      </c>
-      <c r="K3" s="9">
+      <c r="J3" s="7">
+        <f>L3*'Raw data'!$F$25 / 100</f>
+        <v>0.19446506024096391</v>
+      </c>
+      <c r="K3" s="7">
         <f>M3*'Raw data'!$F$25</f>
         <v>2.1783614457831328</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <f>AVERAGE('Raw data'!K3, 'Raw data'!K7) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>0.75903614457831337</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <f>AVERAGE('Raw data'!L3, 'Raw data'!L7) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>8.5025817555938049E-2</v>
       </c>
@@ -781,51 +786,51 @@
       <c r="A4" s="1">
         <v>233</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <f t="shared" ref="B4:B6" si="0">1 - D4 - F4 - 0.07</f>
         <v>0.47211464455348567</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>AVERAGE('Raw data'!G4, 'Raw data'!G8, 'Raw data'!H4, 'Raw data'!H8) / 100 / 'Raw data'!$C$26</f>
         <v>7.4717751996007907E-3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <f>AVERAGE('Raw data'!G4, 'Raw data'!G8)  / 100 / 'Raw data'!$C$26- D4</f>
         <v>5.3772663007319033E-4</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <f>AVERAGE('Raw data'!E4, 'Raw data'!E8) * H4 / (1 - H4) / 100</f>
         <v>0.45041358024691364</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <f>AVERAGE('Raw data'!F4, 'Raw data'!F8) * I4 / (1 - I4) / 100</f>
         <v>8.7755102040816324E-5</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <f>AVERAGE('Raw data'!C4, 'Raw data'!C8) + 0.55 * (1 -  AVERAGE('Raw data'!C4, 'Raw data'!C8))</f>
         <v>0.69625000000000004</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <f>AVERAGE('Raw data'!D4, 'Raw data'!D8)</f>
         <v>0.02</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <f>L4*'Raw data'!$F$25</f>
         <v>6.7467469879518083</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <f>M4*'Raw data'!$F$25</f>
         <v>0.50269879518072291</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <f>AVERAGE('Raw data'!K4, 'Raw data'!K8) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>0.26333907056798628</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="6">
         <f>AVERAGE('Raw data'!L4, 'Raw data'!L8) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>1.9621342512908778E-2</v>
       </c>
@@ -834,51 +839,51 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <f t="shared" si="0"/>
         <v>0.44309871558585973</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <f>AVERAGE('Raw data'!G5, 'Raw data'!G9, 'Raw data'!H5, 'Raw data'!H9) / 100 / 'Raw data'!$C$26</f>
         <v>6.6595974717232132E-3</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <f>AVERAGE('Raw data'!G5, 'Raw data'!G9)  / 100 / 'Raw data'!$C$26- D5</f>
         <v>7.4122588157019345E-4</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <f>AVERAGE('Raw data'!E5, 'Raw data'!E9) * H5 / (1 - H5) / 100</f>
         <v>0.48024168694241709</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <f>AVERAGE('Raw data'!F5, 'Raw data'!F9) * I5 / (1 - I5) / 100</f>
         <v>5.6060606060606054E-5</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <f>AVERAGE('Raw data'!C5, 'Raw data'!C9) + 0.55 * (1 -  AVERAGE('Raw data'!C5, 'Raw data'!C9))</f>
         <v>0.69175000000000009</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <f>AVERAGE('Raw data'!D5, 'Raw data'!D9)</f>
         <v>0.01</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <f>L5*'Raw data'!$F$25</f>
         <v>17.814939759036147</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <f>M5*'Raw data'!$F$25</f>
         <v>2.0901686746987953</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <f>AVERAGE('Raw data'!K5, 'Raw data'!K9) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>0.69535283993115327</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="6">
         <f>AVERAGE('Raw data'!L5, 'Raw data'!L9) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>8.1583476764199664E-2</v>
       </c>
@@ -887,51 +892,51 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <f t="shared" si="0"/>
         <v>0.42394548872180432</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f>AVERAGE('Raw data'!G6, 'Raw data'!G10, 'Raw data'!H6, 'Raw data'!H10) / 100 / 'Raw data'!$C$26</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <f>AVERAGE('Raw data'!G6, 'Raw data'!G10)  / 100 / 'Raw data'!$C$26- D6</f>
         <v>1.2499999999999995E-4</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f>AVERAGE('Raw data'!E6, 'Raw data'!E10) * H6 / (1 - H6) / 100</f>
         <v>0.5058045112781957</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <f>AVERAGE('Raw data'!F6, 'Raw data'!F10) * I6 / (1 - I6) / 100</f>
         <v>4.4897959183673468E-5</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <f>AVERAGE('Raw data'!C6, 'Raw data'!C10) + 0.55 * (1 -  AVERAGE('Raw data'!C6, 'Raw data'!C10))</f>
         <v>0.7007500000000001</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <f>AVERAGE('Raw data'!D6, 'Raw data'!D10)</f>
         <v>0.02</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <f>L6*'Raw data'!$F$25</f>
         <v>25.62</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <f>M6*'Raw data'!$F$25</f>
         <v>3.8628433734939764</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <f>AVERAGE('Raw data'!K6, 'Raw data'!K10) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="6">
         <f>AVERAGE('Raw data'!L6, 'Raw data'!L10) / AVERAGE('Raw data'!$K$6, 'Raw data'!$K$10)</f>
         <v>0.15077452667814115</v>
       </c>
@@ -941,51 +946,51 @@
         <f>'Raw data'!B15</f>
         <v>109</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <f t="shared" ref="B7:B14" si="1">1 - D7 - F7 - 0.07</f>
         <v>0.37583219178082167</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <f>'Raw data'!G15 / 100 / 'Raw data'!$C$26</f>
         <v>2.2499999999999998E-3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <f>'Raw data'!H15 / 100 / 'Raw data'!$C$26</f>
         <v>6.2500000000000001E-4</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f>'Raw data'!E15 * H7 / (1 - H7) / 100</f>
         <v>0.55191780821917835</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <f>'Raw data'!F15 * I7 / (1 - I7) / 100</f>
         <v>9.9174406604747166E-4</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <f>('Raw data'!C15+0.55*(100-'Raw data'!C15)) / 100</f>
         <v>0.6715000000000001</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="6">
         <f>'Raw data'!D15 / 100</f>
         <v>3.1E-2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <f>L7*'Raw data'!$F$25</f>
         <v>16.653000000000002</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <f>M7*'Raw data'!$F$25</f>
         <v>2.3058000000000001</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="6">
         <f>'Raw data'!K15 / 100</f>
         <v>0.65</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="6">
         <f>'Raw data'!L15 / 100</f>
         <v>0.09</v>
       </c>
@@ -995,51 +1000,51 @@
         <f>'Raw data'!B16</f>
         <v>19B</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <f t="shared" si="1"/>
         <v>0.72337947513105738</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <f>'Raw data'!G16 / 100 / 'Raw data'!$C$26</f>
         <v>2.6249999999999997E-3</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <f>'Raw data'!H16 / 100 / 'Raw data'!$C$26</f>
         <v>3.7499999999999995E-4</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f>'Raw data'!E16 * H8 / (1 - H8) / 100</f>
         <v>0.20399552486894265</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <f>'Raw data'!F16 * I8 / (1 - I8) / 100</f>
         <v>1.0101010101010102E-4</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <f>('Raw data'!C16+0.55*(100-'Raw data'!C16)) / 100</f>
         <v>0.6089500000000001</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <f>'Raw data'!D16 / 100</f>
         <v>0.01</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f>L8*'Raw data'!$F$25</f>
         <v>19.727400000000003</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <f>M8*'Raw data'!$F$25</f>
         <v>0.25620000000000004</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <f>'Raw data'!K16 / 100</f>
         <v>0.77</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="6">
         <f>'Raw data'!L16 / 100</f>
         <v>0.01</v>
       </c>
@@ -1049,51 +1054,51 @@
         <f>'Raw data'!B17</f>
         <v>1566</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <f t="shared" si="1"/>
         <v>0.38815561569688734</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <f>'Raw data'!G17 / 100 / 'Raw data'!$C$26</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <f>'Raw data'!H17 / 100 / 'Raw data'!$C$26</f>
         <v>1.6249999999999999E-3</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f>'Raw data'!E17 * H9 / (1 - H9) / 100</f>
         <v>0.52384438430311264</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <f>'Raw data'!F17 * I9 / (1 - I9) / 100</f>
         <v>5.414534288638689E-4</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <f>('Raw data'!C17+0.55*(100-'Raw data'!C17)) / 100</f>
         <v>0.6674500000000001</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="6">
         <f>'Raw data'!D17 / 100</f>
         <v>2.3E-2</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <f>L9*'Raw data'!$F$25</f>
         <v>17.677799999999998</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="7">
         <f>M9*'Raw data'!$F$25</f>
         <v>0.51240000000000008</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="6">
         <f>'Raw data'!K17 / 100</f>
         <v>0.69</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="6">
         <f>'Raw data'!L17 / 100</f>
         <v>0.02</v>
       </c>
@@ -1103,51 +1108,51 @@
         <f>'Raw data'!B18</f>
         <v>327</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <f t="shared" si="1"/>
         <v>0.7325638635210554</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <f>'Raw data'!G18 / 100 / 'Raw data'!$C$26</f>
         <v>6.875E-3</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <f>'Raw data'!H18 / 100 / 'Raw data'!$C$26</f>
         <v>1.1249999999999999E-3</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <f>'Raw data'!E18 * H10 / (1 - H10) / 100</f>
         <v>0.19056113647894471</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <f>'Raw data'!F18 * I10 / (1 - I10) / 100</f>
         <v>1.45748987854251E-4</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <f>('Raw data'!C18+0.55*(100-'Raw data'!C18)) / 100</f>
         <v>0.60580000000000001</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="6">
         <f>'Raw data'!D18 / 100</f>
         <v>1.2E-2</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <f>L10*'Raw data'!$F$25</f>
         <v>17.165400000000002</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <f>M10*'Raw data'!$F$25</f>
         <v>2.0496000000000003</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="6">
         <f>'Raw data'!K18 / 100</f>
         <v>0.67</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="6">
         <f>'Raw data'!L18 / 100</f>
         <v>0.08</v>
       </c>
@@ -1157,51 +1162,51 @@
         <f>'Raw data'!B19</f>
         <v>316</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <f t="shared" si="1"/>
         <v>0.65336248838444178</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <f>'Raw data'!G19 / 100 / 'Raw data'!$C$26</f>
         <v>6.875E-3</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <f>'Raw data'!H19 / 100 / 'Raw data'!$C$26</f>
         <v>3.7499999999999995E-4</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <f>'Raw data'!E19 * H11 / (1 - H11) / 100</f>
         <v>0.26976251161555831</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <f>'Raw data'!F19 * I11 / (1 - I11) / 100</f>
         <v>3.6799184505606529E-4</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <f>('Raw data'!C19+0.55*(100-'Raw data'!C19)) / 100</f>
         <v>0.62335000000000007</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="6">
         <f>'Raw data'!D19 / 100</f>
         <v>1.9E-2</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <f>L11*'Raw data'!$F$25</f>
         <v>19.215</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <f>M11*'Raw data'!$F$25</f>
         <v>1.5371999999999999</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="6">
         <f>'Raw data'!K19 / 100</f>
         <v>0.75</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="6">
         <f>'Raw data'!L19 / 100</f>
         <v>0.06</v>
       </c>
@@ -1211,51 +1216,51 @@
         <f>'Raw data'!B20</f>
         <v>1569</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <f t="shared" si="1"/>
         <v>0.68873476911136988</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <f>'Raw data'!G20 / 100 / 'Raw data'!$C$26</f>
         <v>1.7499999999999998E-2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <f>'Raw data'!H20 / 100 / 'Raw data'!$C$26</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <f>'Raw data'!E20 * H12 / (1 - H12) / 100</f>
         <v>0.22376523088863023</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <f>'Raw data'!F20 * I12 / (1 - I12) / 100</f>
         <v>1.0101010101010102E-4</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <f>('Raw data'!C20+0.55*(100-'Raw data'!C20)) / 100</f>
         <v>0.61345000000000005</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <f>'Raw data'!D20 / 100</f>
         <v>0.01</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <f>L12*'Raw data'!$F$25</f>
         <v>13.834800000000001</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <f>M12*'Raw data'!$F$25</f>
         <v>0.51240000000000008</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="6">
         <f>'Raw data'!K20 / 100</f>
         <v>0.54</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="6">
         <f>'Raw data'!L20 / 100</f>
         <v>0.02</v>
       </c>
@@ -1265,51 +1270,51 @@
         <f>'Raw data'!B21</f>
         <v>1565</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <f t="shared" si="1"/>
         <v>0.47346640658864297</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <f>'Raw data'!G21 / 100 / 'Raw data'!$C$26</f>
         <v>0.02</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <f>'Raw data'!H21 / 100 / 'Raw data'!$C$26</f>
         <v>1.6249999999999999E-3</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <f>'Raw data'!E21 * H13 / (1 - H13) / 100</f>
         <v>0.43653359341135706</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <f>'Raw data'!F21 * I13 / (1 - I13) / 100</f>
         <v>4.0816326530612246E-4</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <f>('Raw data'!C21+0.55*(100-'Raw data'!C21)) / 100</f>
         <v>0.65395000000000014</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <f>'Raw data'!D21 / 100</f>
         <v>0.02</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="7">
         <f>L13*'Raw data'!$F$25</f>
         <v>11.785200000000001</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="7">
         <f>M13*'Raw data'!$F$25</f>
         <v>0.51240000000000008</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="6">
         <f>'Raw data'!K21 / 100</f>
         <v>0.46</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="6">
         <f>'Raw data'!L21 / 100</f>
         <v>0.02</v>
       </c>
@@ -1319,101 +1324,101 @@
         <f>'Raw data'!B22</f>
         <v>1580</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <f t="shared" si="1"/>
         <v>0.6105664150443646</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <f>'Raw data'!G22 / 100 / 'Raw data'!$C$26</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <f>'Raw data'!H22 / 100 / 'Raw data'!$C$26</f>
         <v>2.1250000000000002E-3</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <f>'Raw data'!E22 * H14 / (1 - H14) / 100</f>
         <v>0.26543358495563524</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="6">
         <f>'Raw data'!F22 * I14 / (1 - I14) / 100</f>
         <v>1.0101010101010102E-4</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="6">
         <f>('Raw data'!C22+0.55*(100-'Raw data'!C22)) / 100</f>
         <v>0.62245000000000017</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="6">
         <f>'Raw data'!D22 / 100</f>
         <v>0.01</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <f>L14*'Raw data'!$F$25</f>
         <v>4.8677999999999999</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="7">
         <f>M14*'Raw data'!$F$25</f>
         <v>0.25620000000000004</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="6">
         <f>'Raw data'!K22 / 100</f>
         <v>0.19</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="6">
         <f>'Raw data'!L22 / 100</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="8">
+        <v>63</v>
+      </c>
+      <c r="B15" s="6">
         <f>1-D15-F15-0.07</f>
         <v>0.70225000000000004</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <f>D6</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="6">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <f>0.091 / 0.4</f>
         <v>0.22749999999999998</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="6">
         <v>1E-3</v>
       </c>
-      <c r="H15" s="8">
-        <f>0.4</f>
-        <v>0.4</v>
-      </c>
-      <c r="I15" s="8">
+      <c r="H15" s="6">
+        <f>0.6</f>
+        <v>0.6</v>
+      </c>
+      <c r="I15" s="6">
         <f>'Raw data'!D23 / 100</f>
         <v>0</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <f>L15*'Raw data'!$F$25</f>
         <v>45.56</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <f>M15*'Raw data'!$F$25</f>
         <v>0</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="6">
         <f>'Raw data'!F27/'Raw data'!F25</f>
         <v>1.7782982045277127</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="6">
         <f>'Raw data'!L23 / 100</f>
         <v>0</v>
       </c>
@@ -1436,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC404B78-4659-4EF1-B71B-6CB09BD44206}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,36 +1462,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>36</v>
       </c>
@@ -1519,7 +1524,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
@@ -1557,7 +1562,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1">
         <v>233</v>
       </c>
@@ -1593,7 +1598,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1634,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1665,7 +1670,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B7" t="s">
@@ -1703,7 +1708,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>233</v>
       </c>
@@ -1739,7 +1744,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -1775,7 +1780,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -1811,36 +1816,36 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -1873,7 +1878,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B14" t="s">
@@ -1907,7 +1912,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1">
         <v>109</v>
       </c>
@@ -1939,7 +1944,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" t="s">
         <v>49</v>
       </c>
@@ -1971,7 +1976,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1">
         <v>1566</v>
       </c>
@@ -2003,7 +2008,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="1">
         <v>327</v>
       </c>
@@ -2035,7 +2040,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1">
         <v>316</v>
       </c>
@@ -2067,7 +2072,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1">
         <v>1569</v>
       </c>
@@ -2099,7 +2104,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1">
         <v>1565</v>
       </c>
@@ -2131,7 +2136,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="4">
         <v>1580</v>
       </c>
@@ -2168,10 +2173,10 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" t="s">
         <v>55</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2216,7 +2221,7 @@
         <v>52</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2228,11 +2233,15 @@
         <v>45.56</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A3:A6"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -2246,10 +2255,6 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1" xr:uid="{72262BB2-DE02-4A6B-8EDA-4BD7DB0E8320}"/>

</xml_diff>

<commit_message>
fix units of area
</commit_message>
<xml_diff>
--- a/biorefineries/cane/data/cane_composition_data.xlsx
+++ b/biorefineries/cane/data/cane_composition_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\biosteam\Bioindustrial-Park\biorefineries\cane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB502FE-AF9B-422E-9690-A28741E49167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE3F710-5C90-4E93-817F-3C142B53F413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A4D5F0FC-4525-4FC3-8D16-C4CDE02F4321}"/>
   </bookViews>
@@ -235,10 +235,10 @@
     <t>Dry biomass yield (WT)</t>
   </si>
   <si>
-    <t>Biomass yield (dry MT/hc)</t>
-  </si>
-  <si>
     <t>Yield (dry MT/hc)</t>
+  </si>
+  <si>
+    <t>Biomass yield (dry MT/ha)</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +682,7 @@
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8" t="s">
@@ -2173,7 +2173,7 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
         <v>55</v>
@@ -2238,6 +2238,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K1:L1"/>
@@ -2254,7 +2255,6 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1" xr:uid="{72262BB2-DE02-4A6B-8EDA-4BD7DB0E8320}"/>

</xml_diff>

<commit_message>
work on microbial oilplots
</commit_message>
<xml_diff>
--- a/biorefineries/cane/data/cane_composition_data.xlsx
+++ b/biorefineries/cane/data/cane_composition_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\biosteam\Bioindustrial-Park\biorefineries\cane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE3F710-5C90-4E93-817F-3C142B53F413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9C5E28-916D-4F70-9EFA-60A406F87F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A4D5F0FC-4525-4FC3-8D16-C4CDE02F4321}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Summarized" sheetId="1" r:id="rId1"/>
     <sheet name="Raw data" sheetId="3" r:id="rId2"/>
     <sheet name="Raw data from graph" sheetId="2" r:id="rId3"/>
+    <sheet name="NotUsed" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -235,10 +236,10 @@
     <t>Dry biomass yield (WT)</t>
   </si>
   <si>
-    <t>Yield (dry MT/hc)</t>
-  </si>
-  <si>
     <t>Biomass yield (dry MT/ha)</t>
+  </si>
+  <si>
+    <t>Yield (dry MT/ha)</t>
   </si>
 </sst>
 </file>
@@ -631,7 +632,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -639,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A5991C-2AB0-423D-B833-4415103D81DC}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +683,7 @@
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8" t="s">
@@ -1055,7 +1056,7 @@
         <v>1566</v>
       </c>
       <c r="B9" s="6">
-        <f t="shared" si="1"/>
+        <f>1 - D9 - F9 - 0.07</f>
         <v>0.38815561569688734</v>
       </c>
       <c r="C9" s="6">
@@ -1271,7 +1272,7 @@
         <v>1565</v>
       </c>
       <c r="B13" s="6">
-        <f t="shared" si="1"/>
+        <f>1 - D13 - F13 - 0.07</f>
         <v>0.47346640658864297</v>
       </c>
       <c r="C13" s="6">
@@ -1371,56 +1372,6 @@
       <c r="M14" s="6">
         <f>'Raw data'!L22 / 100</f>
         <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="6">
-        <f>1-D15-F15-0.07</f>
-        <v>0.70225000000000004</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="D15" s="6">
-        <f>D6</f>
-        <v>2.5000000000000001E-4</v>
-      </c>
-      <c r="E15" s="6">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="F15" s="6">
-        <f>0.091 / 0.4</f>
-        <v>0.22749999999999998</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="H15" s="6">
-        <f>0.6</f>
-        <v>0.6</v>
-      </c>
-      <c r="I15" s="6">
-        <f>'Raw data'!D23 / 100</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <f>L15*'Raw data'!$F$25</f>
-        <v>45.56</v>
-      </c>
-      <c r="K15" s="7">
-        <f>M15*'Raw data'!$F$25</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
-        <f>'Raw data'!F27/'Raw data'!F25</f>
-        <v>1.7782982045277127</v>
-      </c>
-      <c r="M15" s="6">
-        <f>'Raw data'!L23 / 100</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1393,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,7 +1403,7 @@
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" customWidth="1"/>
     <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5546875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -2173,7 +2124,7 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G24" t="s">
         <v>55</v>
@@ -2238,7 +2189,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K1:L1"/>
@@ -2255,6 +2205,7 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1" xr:uid="{72262BB2-DE02-4A6B-8EDA-4BD7DB0E8320}"/>
@@ -2427,4 +2378,69 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591B773F-25A7-4E67-BA2B-10E105F214E0}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="6">
+        <f>1-D1-F1-0.07</f>
+        <v>0.70225000000000004</v>
+      </c>
+      <c r="C1" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D1" s="6">
+        <f>Summarized!D6</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="E1" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F1" s="6">
+        <f>0.091 / 0.4</f>
+        <v>0.22749999999999998</v>
+      </c>
+      <c r="G1" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="H1" s="6">
+        <f>0.6</f>
+        <v>0.6</v>
+      </c>
+      <c r="I1" s="6">
+        <f>'Raw data'!D23 / 100</f>
+        <v>0</v>
+      </c>
+      <c r="J1" s="7">
+        <f>L1*'Raw data'!$F$25</f>
+        <v>45.56</v>
+      </c>
+      <c r="K1" s="7">
+        <f>M1*'Raw data'!$F$25</f>
+        <v>0</v>
+      </c>
+      <c r="L1" s="6">
+        <f>'Raw data'!F27/'Raw data'!F25</f>
+        <v>1.7782982045277127</v>
+      </c>
+      <c r="M1" s="6">
+        <f>'Raw data'!L23 / 100</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more features for cane publication
</commit_message>
<xml_diff>
--- a/biorefineries/cane/data/cane_composition_data.xlsx
+++ b/biorefineries/cane/data/cane_composition_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\biosteam\Bioindustrial-Park\biorefineries\cane\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9C5E28-916D-4F70-9EFA-60A406F87F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B3368C-5CCC-4611-8523-1F97D4BD66EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A4D5F0FC-4525-4FC3-8D16-C4CDE02F4321}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="13800" activeTab="1" xr2:uid="{A4D5F0FC-4525-4FC3-8D16-C4CDE02F4321}"/>
   </bookViews>
   <sheets>
     <sheet name="Summarized" sheetId="1" r:id="rId1"/>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A5991C-2AB0-423D-B833-4415103D81DC}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +949,7 @@
       </c>
       <c r="B7" s="6">
         <f t="shared" ref="B7:B14" si="1">1 - D7 - F7 - 0.07</f>
-        <v>0.37583219178082167</v>
+        <v>0.55776065449010637</v>
       </c>
       <c r="C7" s="6">
         <f>0</f>
@@ -965,7 +965,7 @@
       </c>
       <c r="F7" s="6">
         <f>'Raw data'!E15 * H7 / (1 - H7) / 100</f>
-        <v>0.55191780821917835</v>
+        <v>0.36998934550989371</v>
       </c>
       <c r="G7" s="6">
         <f>'Raw data'!F15 * I7 / (1 - I7) / 100</f>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B8" s="6">
         <f t="shared" si="1"/>
-        <v>0.72337947513105738</v>
+        <v>0.65330467651195478</v>
       </c>
       <c r="C8" s="6">
         <f>0</f>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="F8" s="6">
         <f>'Raw data'!E16 * H8 / (1 - H8) / 100</f>
-        <v>0.20399552486894265</v>
+        <v>0.27407032348804511</v>
       </c>
       <c r="G8" s="6">
         <f>'Raw data'!F16 * I8 / (1 - I8) / 100</f>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B9" s="6">
         <f>1 - D9 - F9 - 0.07</f>
-        <v>0.38815561569688734</v>
+        <v>0.54470681100586349</v>
       </c>
       <c r="C9" s="6">
         <f>0</f>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="F9" s="6">
         <f>'Raw data'!E17 * H9 / (1 - H9) / 100</f>
-        <v>0.52384438430311264</v>
+        <v>0.36729318899413643</v>
       </c>
       <c r="G9" s="6">
         <f>'Raw data'!F17 * I9 / (1 - I9) / 100</f>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B10" s="6">
         <f t="shared" si="1"/>
-        <v>0.7325638635210554</v>
+        <v>0.65726147894469822</v>
       </c>
       <c r="C10" s="6">
         <f>0</f>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="F10" s="6">
         <f>'Raw data'!E18 * H10 / (1 - H10) / 100</f>
-        <v>0.19056113647894471</v>
+        <v>0.26586352105530187</v>
       </c>
       <c r="G10" s="6">
         <f>'Raw data'!F18 * I10 / (1 - I10) / 100</f>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B11" s="6">
         <f t="shared" si="1"/>
-        <v>0.65336248838444178</v>
+        <v>0.60371294636930828</v>
       </c>
       <c r="C11" s="6">
         <f>0</f>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F11" s="6">
         <f>'Raw data'!E19 * H11 / (1 - H11) / 100</f>
-        <v>0.26976251161555831</v>
+        <v>0.31941205363069175</v>
       </c>
       <c r="G11" s="6">
         <f>'Raw data'!F19 * I11 / (1 - I11) / 100</f>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B12" s="6">
         <f t="shared" si="1"/>
-        <v>0.68873476911136988</v>
+        <v>0.63160322079937914</v>
       </c>
       <c r="C12" s="6">
         <f>0</f>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="F12" s="6">
         <f>'Raw data'!E20 * H12 / (1 - H12) / 100</f>
-        <v>0.22376523088863023</v>
+        <v>0.28089677920062089</v>
       </c>
       <c r="G12" s="6">
         <f>'Raw data'!F20 * I12 / (1 - I12) / 100</f>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B13" s="6">
         <f>1 - D13 - F13 - 0.07</f>
-        <v>0.47346640658864297</v>
+        <v>0.57551322063285637</v>
       </c>
       <c r="C13" s="6">
         <f>0</f>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F13" s="6">
         <f>'Raw data'!E21 * H13 / (1 - H13) / 100</f>
-        <v>0.43653359341135706</v>
+        <v>0.33448677936714366</v>
       </c>
       <c r="G13" s="6">
         <f>'Raw data'!F21 * I13 / (1 - I13) / 100</f>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="B14" s="6">
         <f t="shared" si="1"/>
-        <v>0.6105664150443646</v>
+        <v>0.57759329890080746</v>
       </c>
       <c r="C14" s="6">
         <f>0</f>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="F14" s="6">
         <f>'Raw data'!E22 * H14 / (1 - H14) / 100</f>
-        <v>0.26543358495563524</v>
+        <v>0.29840670109919243</v>
       </c>
       <c r="G14" s="6">
         <f>'Raw data'!F22 * I14 / (1 - I14) / 100</f>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC404B78-4659-4EF1-B71B-6CB09BD44206}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1842,7 +1842,7 @@
         <v>1.3</v>
       </c>
       <c r="E14">
-        <v>21.2</v>
+        <v>21.7</v>
       </c>
       <c r="F14">
         <v>1.3</v>
@@ -1874,7 +1874,7 @@
         <v>3.1</v>
       </c>
       <c r="E15">
-        <v>27</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F15">
         <v>3.1</v>
@@ -1906,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>13.1</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1938,7 +1938,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E17">
-        <v>26.1</v>
+        <v>18.3</v>
       </c>
       <c r="F17">
         <v>2.2999999999999998</v>
@@ -1970,7 +1970,7 @@
         <v>1.2</v>
       </c>
       <c r="E18">
-        <v>12.4</v>
+        <v>17.3</v>
       </c>
       <c r="F18">
         <v>1.2</v>
@@ -2002,7 +2002,7 @@
         <v>1.9</v>
       </c>
       <c r="E19">
-        <v>16.3</v>
+        <v>19.3</v>
       </c>
       <c r="F19">
         <v>1.9</v>
@@ -2034,7 +2034,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>14.1</v>
+        <v>17.7</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2066,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>23.1</v>
+        <v>17.7</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>16.100000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2189,6 +2189,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K1:L1"/>
@@ -2205,7 +2206,6 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1" xr:uid="{72262BB2-DE02-4A6B-8EDA-4BD7DB0E8320}"/>

</xml_diff>

<commit_message>
important updates to model
</commit_message>
<xml_diff>
--- a/biorefineries/cane/data/cane_composition_data.xlsx
+++ b/biorefineries/cane/data/cane_composition_data.xlsx
@@ -1091,13 +1091,13 @@
         <v>0.001</v>
       </c>
       <c r="J16" t="n">
-        <v>20.64918974810691</v>
+        <v>18.16889414492636</v>
       </c>
       <c r="K16" t="n">
         <v>0.001</v>
       </c>
       <c r="L16" t="n">
-        <v>0.8059793032047973</v>
+        <v>0.7091683897317078</v>
       </c>
       <c r="M16" t="n">
         <v>0.001</v>

</xml_diff>